<commit_message>
File template Change For Airport Station
</commit_message>
<xml_diff>
--- a/src/assets/static-content/AirportStation.xlsx
+++ b/src/assets/static-content/AirportStation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>IATA Code</t>
   </si>
@@ -25,16 +25,10 @@
     <t>City</t>
   </si>
   <si>
-    <t>AAA</t>
+    <t>Country</t>
   </si>
   <si>
-    <t>Allpey</t>
-  </si>
-  <si>
-    <t>BBB</t>
-  </si>
-  <si>
-    <t>BBD Bag</t>
+    <t>Timezone</t>
   </si>
 </sst>
 </file>
@@ -376,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,9 +381,10 @@
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,27 +394,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>